<commit_message>
Finalização do Documento de Requisito
</commit_message>
<xml_diff>
--- a/gestao_projetos/Matriz Rastreabilidade de Requisitos - Modelo.xlsx
+++ b/gestao_projetos/Matriz Rastreabilidade de Requisitos - Modelo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\ProjetoIntegrador\gestao_projetos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA8874D-7AD2-476C-8A12-C2D080C743C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8092EC2C-FF10-47B6-B8DF-D7CDC85ABAB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{653CD9F3-5A9F-41BF-9894-9B82D1FDAD46}"/>
   </bookViews>
@@ -354,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -386,6 +386,15 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -393,6 +402,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -434,22 +446,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -768,7 +765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B72DBFA-E277-44B9-B1E7-DA38DDEFE762}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -783,46 +780,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="29"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="13"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:6" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="13"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -834,11 +831,11 @@
       <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="13"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
@@ -867,7 +864,7 @@
       <c r="A8" s="31">
         <v>1</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -887,19 +884,19 @@
       <c r="A9" s="31">
         <v>2</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -907,19 +904,19 @@
       <c r="A10" s="31">
         <v>3</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -927,19 +924,19 @@
       <c r="A11" s="31">
         <v>4</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -947,19 +944,19 @@
       <c r="A12" s="31">
         <v>5</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -967,19 +964,19 @@
       <c r="A13" s="31">
         <v>6</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -990,73 +987,68 @@
       <c r="A15" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="13"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="16"/>
     </row>
     <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="13"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="16"/>
     </row>
     <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="11"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="26"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="30"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="24"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="28"/>
     </row>
     <row r="19" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="18"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="22"/>
     </row>
     <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="21"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="D5:F5"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="A19:A20"/>
@@ -1064,6 +1056,11 @@
     <mergeCell ref="C19:F20"/>
     <mergeCell ref="A18:F18"/>
     <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="D5:F5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>